<commit_message>
Pharmacy Cleaning (Fixed Steps # for individual hospitals)
</commit_message>
<xml_diff>
--- a/IS447/System/Data/Pharmacy Dept/MNH TTO Data/MNH Wards.xlsx
+++ b/IS447/System/Data/Pharmacy Dept/MNH TTO Data/MNH Wards.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherminliam/Documents/School Work/IS447/IS447---Smart-Healthcare/IS447/System/Data/Pharmacy Dept/MNH TTO Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB52D86E-BFE3-FD4F-AFE4-1D45D4D6141D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" tabRatio="689" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16400" tabRatio="689" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W2" sheetId="1" r:id="rId1"/>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="60">
   <si>
     <t>Ward</t>
   </si>
@@ -206,12 +212,15 @@
   </si>
   <si>
     <t>6Peds</t>
+  </si>
+  <si>
+    <t>NICU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,8 +250,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,176 +273,176 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B37" totalsRowShown="0">
-  <autoFilter ref="A1:B37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B37" totalsRowShown="0">
+  <autoFilter ref="A1:B37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1457" displayName="Table1457" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table1457" displayName="Table1457" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14578" displayName="Table14578" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table14578" displayName="Table14578" ref="A1:B35" totalsRowShown="0">
+  <autoFilter ref="A1:B35" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A1:B27" totalsRowShown="0">
-  <autoFilter ref="A1:B27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table1456" displayName="Table1456" ref="A1:B27" totalsRowShown="0">
+  <autoFilter ref="A1:B27" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table145" displayName="Table145" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:B31" totalsRowShown="0">
-  <autoFilter ref="A1:B31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table14" displayName="Table14" ref="A1:B31" totalsRowShown="0">
+  <autoFilter ref="A1:B31" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:B18" totalsRowShown="0">
-  <autoFilter ref="A1:B18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table13" displayName="Table13" ref="A1:B18" totalsRowShown="0">
+  <autoFilter ref="A1:B18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1315" displayName="Table1315" ref="A1:B18" totalsRowShown="0">
-  <autoFilter ref="A1:B18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table1315" displayName="Table1315" ref="A1:B18" totalsRowShown="0">
+  <autoFilter ref="A1:B18" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table112" displayName="Table112" ref="A1:B21" totalsRowShown="0">
-  <autoFilter ref="A1:B21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table112" displayName="Table112" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1121314" displayName="Table1121314" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1121314" displayName="Table1121314" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table11213" displayName="Table11213" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table11213" displayName="Table11213" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1457910111617" displayName="Table1457910111617" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1457910111617" displayName="Table1457910111617" ref="A1:B20" totalsRowShown="0">
+  <autoFilter ref="A1:B20" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table14579101116" displayName="Table14579101116" ref="A1:B21" totalsRowShown="0">
-  <autoFilter ref="A1:B21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table14579101116" displayName="Table14579101116" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table145791011" displayName="Table145791011" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table145791011" displayName="Table145791011" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1457910" displayName="Table1457910" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table1457910" displayName="Table1457910" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table14579" displayName="Table14579" ref="A1:B33" totalsRowShown="0">
-  <autoFilter ref="A1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table14579" displayName="Table14579" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Room No"/>
-    <tableColumn id="2" name="Ward"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Room No"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Ward"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -512,6 +524,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -547,6 +576,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,19 +768,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -742,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>201</v>
       </c>
@@ -750,7 +796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>202</v>
       </c>
@@ -758,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>203</v>
       </c>
@@ -766,7 +812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>204</v>
       </c>
@@ -774,7 +820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>205</v>
       </c>
@@ -782,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>206</v>
       </c>
@@ -790,7 +836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>207</v>
       </c>
@@ -798,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>208</v>
       </c>
@@ -806,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>209</v>
       </c>
@@ -814,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>210</v>
       </c>
@@ -822,7 +868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>211</v>
       </c>
@@ -830,7 +876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>212</v>
       </c>
@@ -838,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>213</v>
       </c>
@@ -846,7 +892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>214</v>
       </c>
@@ -854,7 +900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>215</v>
       </c>
@@ -862,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>216</v>
       </c>
@@ -870,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>217</v>
       </c>
@@ -878,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>218</v>
       </c>
@@ -886,7 +932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>219</v>
       </c>
@@ -894,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>220</v>
       </c>
@@ -902,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>260</v>
       </c>
@@ -910,7 +956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>261</v>
       </c>
@@ -918,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>262</v>
       </c>
@@ -926,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>263</v>
       </c>
@@ -934,7 +980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>265</v>
       </c>
@@ -942,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>266</v>
       </c>
@@ -950,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>267</v>
       </c>
@@ -958,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>268</v>
       </c>
@@ -966,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>269</v>
       </c>
@@ -974,7 +1020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>270</v>
       </c>
@@ -982,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>271</v>
       </c>
@@ -990,7 +1036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>272</v>
       </c>
@@ -998,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>273</v>
       </c>
@@ -1006,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>275</v>
       </c>
@@ -1014,7 +1060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>276</v>
       </c>
@@ -1022,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>277</v>
       </c>
@@ -1039,19 +1085,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1059,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>901</v>
       </c>
@@ -1067,7 +1113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>902</v>
       </c>
@@ -1075,7 +1121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>903</v>
       </c>
@@ -1083,7 +1129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>904</v>
       </c>
@@ -1091,7 +1137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>905</v>
       </c>
@@ -1099,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>906</v>
       </c>
@@ -1107,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>907</v>
       </c>
@@ -1115,7 +1161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>908</v>
       </c>
@@ -1123,7 +1169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>909</v>
       </c>
@@ -1131,7 +1177,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>910</v>
       </c>
@@ -1139,7 +1185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>911</v>
       </c>
@@ -1147,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>912</v>
       </c>
@@ -1155,7 +1201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>913</v>
       </c>
@@ -1163,7 +1209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>914</v>
       </c>
@@ -1171,7 +1217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>915</v>
       </c>
@@ -1179,7 +1225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>916</v>
       </c>
@@ -1187,7 +1233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>917</v>
       </c>
@@ -1195,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>918</v>
       </c>
@@ -1203,7 +1249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>919</v>
       </c>
@@ -1211,7 +1257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>920</v>
       </c>
@@ -1219,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>921</v>
       </c>
@@ -1227,7 +1273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>922</v>
       </c>
@@ -1235,7 +1281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>923</v>
       </c>
@@ -1243,7 +1289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>924</v>
       </c>
@@ -1251,7 +1297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>925</v>
       </c>
@@ -1259,7 +1305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>926</v>
       </c>
@@ -1267,7 +1313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>927</v>
       </c>
@@ -1275,7 +1321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>928</v>
       </c>
@@ -1283,7 +1329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>929</v>
       </c>
@@ -1291,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>930</v>
       </c>
@@ -1299,7 +1345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>931</v>
       </c>
@@ -1307,7 +1353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>932</v>
       </c>
@@ -1324,19 +1370,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A17" zoomScale="136" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1344,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1352,7 +1398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1368,7 +1414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1384,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1392,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1400,7 +1446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1408,7 +1454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1416,7 +1462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1424,7 +1470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1432,7 +1478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1440,7 +1486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1456,7 +1502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1464,7 +1510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1472,7 +1518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1488,7 +1534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1496,7 +1542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1504,7 +1550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1512,7 +1558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1520,7 +1566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1528,7 +1574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1536,7 +1582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1544,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1552,7 +1598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1560,7 +1606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1568,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1576,7 +1622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1584,7 +1630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1592,11 +1638,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>933</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>937</v>
+      </c>
+      <c r="B35" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1609,19 +1671,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1629,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1637,7 +1699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1645,7 +1707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1653,7 +1715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1661,7 +1723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1669,7 +1731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1677,7 +1739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1685,7 +1747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1693,7 +1755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1701,7 +1763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1709,7 +1771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1717,7 +1779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1725,7 +1787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -1733,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -1741,7 +1803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -1749,7 +1811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -1757,7 +1819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -1765,7 +1827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1018</v>
       </c>
@@ -1773,7 +1835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1019</v>
       </c>
@@ -1781,7 +1843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1020</v>
       </c>
@@ -1789,7 +1851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1021</v>
       </c>
@@ -1797,7 +1859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1022</v>
       </c>
@@ -1805,7 +1867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1023</v>
       </c>
@@ -1813,7 +1875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1024</v>
       </c>
@@ -1821,7 +1883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1025</v>
       </c>
@@ -1829,7 +1891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1026</v>
       </c>
@@ -1846,19 +1908,19 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1866,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1101</v>
       </c>
@@ -1874,7 +1936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1102</v>
       </c>
@@ -1882,7 +1944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1103</v>
       </c>
@@ -1890,7 +1952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1104</v>
       </c>
@@ -1898,7 +1960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1105</v>
       </c>
@@ -1906,7 +1968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1106</v>
       </c>
@@ -1914,7 +1976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1107</v>
       </c>
@@ -1922,7 +1984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1108</v>
       </c>
@@ -1930,7 +1992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1109</v>
       </c>
@@ -1938,7 +2000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1110</v>
       </c>
@@ -1946,7 +2008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1111</v>
       </c>
@@ -1954,7 +2016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1112</v>
       </c>
@@ -1962,7 +2024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1113</v>
       </c>
@@ -1970,7 +2032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1114</v>
       </c>
@@ -1978,7 +2040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1115</v>
       </c>
@@ -1986,7 +2048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1116</v>
       </c>
@@ -1994,7 +2056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1117</v>
       </c>
@@ -2002,7 +2064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1118</v>
       </c>
@@ -2010,7 +2072,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1119</v>
       </c>
@@ -2018,7 +2080,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1120</v>
       </c>
@@ -2026,7 +2088,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1121</v>
       </c>
@@ -2034,7 +2096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1122</v>
       </c>
@@ -2042,7 +2104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1123</v>
       </c>
@@ -2050,7 +2112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1124</v>
       </c>
@@ -2058,7 +2120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1125</v>
       </c>
@@ -2066,7 +2128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1126</v>
       </c>
@@ -2074,7 +2136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1127</v>
       </c>
@@ -2082,7 +2144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1128</v>
       </c>
@@ -2090,7 +2152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1129</v>
       </c>
@@ -2098,7 +2160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1130</v>
       </c>
@@ -2106,7 +2168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1131</v>
       </c>
@@ -2114,7 +2176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1132</v>
       </c>
@@ -2131,19 +2193,19 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2151,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1201</v>
       </c>
@@ -2159,7 +2221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1202</v>
       </c>
@@ -2167,7 +2229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1203</v>
       </c>
@@ -2175,7 +2237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1204</v>
       </c>
@@ -2183,7 +2245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1205</v>
       </c>
@@ -2191,7 +2253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1206</v>
       </c>
@@ -2199,7 +2261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1207</v>
       </c>
@@ -2207,7 +2269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1208</v>
       </c>
@@ -2215,7 +2277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1209</v>
       </c>
@@ -2223,7 +2285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1210</v>
       </c>
@@ -2231,7 +2293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1211</v>
       </c>
@@ -2239,7 +2301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1212</v>
       </c>
@@ -2247,7 +2309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1213</v>
       </c>
@@ -2255,7 +2317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1214</v>
       </c>
@@ -2263,7 +2325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1215</v>
       </c>
@@ -2271,7 +2333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1216</v>
       </c>
@@ -2279,7 +2341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1217</v>
       </c>
@@ -2287,7 +2349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1218</v>
       </c>
@@ -2295,7 +2357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1219</v>
       </c>
@@ -2303,7 +2365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1220</v>
       </c>
@@ -2311,7 +2373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1221</v>
       </c>
@@ -2319,7 +2381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1222</v>
       </c>
@@ -2327,7 +2389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1223</v>
       </c>
@@ -2335,7 +2397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1224</v>
       </c>
@@ -2343,7 +2405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1225</v>
       </c>
@@ -2351,7 +2413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1226</v>
       </c>
@@ -2359,7 +2421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1227</v>
       </c>
@@ -2367,7 +2429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1228</v>
       </c>
@@ -2375,7 +2437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1229</v>
       </c>
@@ -2383,7 +2445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1230</v>
       </c>
@@ -2400,20 +2462,20 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2421,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1301</v>
       </c>
@@ -2429,7 +2491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1302</v>
       </c>
@@ -2437,7 +2499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1303</v>
       </c>
@@ -2445,7 +2507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1304</v>
       </c>
@@ -2453,7 +2515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1305</v>
       </c>
@@ -2461,7 +2523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1306</v>
       </c>
@@ -2469,7 +2531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1307</v>
       </c>
@@ -2477,7 +2539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1308</v>
       </c>
@@ -2485,7 +2547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1309</v>
       </c>
@@ -2493,7 +2555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1310</v>
       </c>
@@ -2501,7 +2563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1311</v>
       </c>
@@ -2509,7 +2571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1312</v>
       </c>
@@ -2517,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1313</v>
       </c>
@@ -2525,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1314</v>
       </c>
@@ -2533,7 +2595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1315</v>
       </c>
@@ -2541,7 +2603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1316</v>
       </c>
@@ -2549,7 +2611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1317</v>
       </c>
@@ -2566,20 +2628,20 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2587,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2595,7 +2657,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2603,7 +2665,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2611,7 +2673,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2619,7 +2681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2627,7 +2689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2635,7 +2697,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2643,7 +2705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2651,7 +2713,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2659,7 +2721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2667,7 +2729,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2675,7 +2737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2683,7 +2745,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2691,7 +2753,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2699,7 +2761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2707,7 +2769,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2715,7 +2777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2732,19 +2794,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A9" zoomScale="139" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2752,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>301</v>
       </c>
@@ -2760,7 +2822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>302</v>
       </c>
@@ -2768,7 +2830,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>303</v>
       </c>
@@ -2776,7 +2838,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>304</v>
       </c>
@@ -2784,7 +2846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>305</v>
       </c>
@@ -2792,7 +2854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>306</v>
       </c>
@@ -2800,7 +2862,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>307</v>
       </c>
@@ -2808,7 +2870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>308</v>
       </c>
@@ -2816,7 +2878,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>309</v>
       </c>
@@ -2824,7 +2886,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>310</v>
       </c>
@@ -2832,7 +2894,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>311</v>
       </c>
@@ -2840,7 +2902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>312</v>
       </c>
@@ -2848,7 +2910,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>313</v>
       </c>
@@ -2856,7 +2918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>314</v>
       </c>
@@ -2864,7 +2926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>315</v>
       </c>
@@ -2872,7 +2934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>316</v>
       </c>
@@ -2880,7 +2942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>317</v>
       </c>
@@ -2888,7 +2950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>318</v>
       </c>
@@ -2896,7 +2958,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>319</v>
       </c>
@@ -2904,12 +2966,108 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>320</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>361</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>362</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>363</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>364</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>365</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>366</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>367</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>368</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>369</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>370</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>371</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>372</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2921,20 +3079,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="157" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2942,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>321</v>
       </c>
@@ -2950,7 +3108,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>322</v>
       </c>
@@ -2958,7 +3116,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>323</v>
       </c>
@@ -2966,7 +3124,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>324</v>
       </c>
@@ -2974,7 +3132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>325</v>
       </c>
@@ -2982,7 +3140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>340</v>
       </c>
@@ -2999,19 +3157,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3019,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>326</v>
       </c>
@@ -3027,7 +3185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>327</v>
       </c>
@@ -3035,7 +3193,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>328</v>
       </c>
@@ -3043,7 +3201,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>329</v>
       </c>
@@ -3051,7 +3209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>330</v>
       </c>
@@ -3059,7 +3217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>331</v>
       </c>
@@ -3067,7 +3225,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>332</v>
       </c>
@@ -3075,7 +3233,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>333</v>
       </c>
@@ -3083,7 +3241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>338</v>
       </c>
@@ -3091,7 +3249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>339</v>
       </c>
@@ -3108,19 +3266,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3128,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>460</v>
       </c>
@@ -3136,7 +3294,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>461</v>
       </c>
@@ -3144,7 +3302,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>462</v>
       </c>
@@ -3152,7 +3310,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>463</v>
       </c>
@@ -3160,7 +3318,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>465</v>
       </c>
@@ -3168,7 +3326,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>466</v>
       </c>
@@ -3176,7 +3334,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>467</v>
       </c>
@@ -3184,7 +3342,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>468</v>
       </c>
@@ -3192,7 +3350,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>469</v>
       </c>
@@ -3200,7 +3358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>470</v>
       </c>
@@ -3208,7 +3366,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>471</v>
       </c>
@@ -3216,7 +3374,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>472</v>
       </c>
@@ -3224,7 +3382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>473</v>
       </c>
@@ -3232,7 +3390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>475</v>
       </c>
@@ -3240,7 +3398,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>476</v>
       </c>
@@ -3248,7 +3406,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>477</v>
       </c>
@@ -3256,7 +3414,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>478</v>
       </c>
@@ -3264,7 +3422,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>479</v>
       </c>
@@ -3272,7 +3430,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>480</v>
       </c>
@@ -3289,19 +3447,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3309,7 +3467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>401</v>
       </c>
@@ -3317,7 +3475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>402</v>
       </c>
@@ -3325,7 +3483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>403</v>
       </c>
@@ -3333,7 +3491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>405</v>
       </c>
@@ -3341,7 +3499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>406</v>
       </c>
@@ -3349,7 +3507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>407</v>
       </c>
@@ -3357,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>408</v>
       </c>
@@ -3365,7 +3523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>409</v>
       </c>
@@ -3373,7 +3531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>410</v>
       </c>
@@ -3381,7 +3539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>411</v>
       </c>
@@ -3389,7 +3547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>412</v>
       </c>
@@ -3397,7 +3555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>413</v>
       </c>
@@ -3405,7 +3563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>415</v>
       </c>
@@ -3413,7 +3571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>416</v>
       </c>
@@ -3421,7 +3579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>417</v>
       </c>
@@ -3429,7 +3587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>418</v>
       </c>
@@ -3437,7 +3595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>419</v>
       </c>
@@ -3445,7 +3603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>420</v>
       </c>
@@ -3453,7 +3611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>421</v>
       </c>
@@ -3461,7 +3619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>422</v>
       </c>
@@ -3478,19 +3636,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3498,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>601</v>
       </c>
@@ -3506,7 +3664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>602</v>
       </c>
@@ -3514,7 +3672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>603</v>
       </c>
@@ -3522,7 +3680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>604</v>
       </c>
@@ -3530,7 +3688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>605</v>
       </c>
@@ -3538,7 +3696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>606</v>
       </c>
@@ -3546,7 +3704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>607</v>
       </c>
@@ -3554,7 +3712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>608</v>
       </c>
@@ -3562,7 +3720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>609</v>
       </c>
@@ -3570,7 +3728,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>610</v>
       </c>
@@ -3578,7 +3736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>611</v>
       </c>
@@ -3586,7 +3744,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>612</v>
       </c>
@@ -3594,7 +3752,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>613</v>
       </c>
@@ -3602,7 +3760,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>614</v>
       </c>
@@ -3610,7 +3768,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>615</v>
       </c>
@@ -3618,7 +3776,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>616</v>
       </c>
@@ -3626,7 +3784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>617</v>
       </c>
@@ -3634,7 +3792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>618</v>
       </c>
@@ -3642,7 +3800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>619</v>
       </c>
@@ -3650,7 +3808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>620</v>
       </c>
@@ -3658,7 +3816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>621</v>
       </c>
@@ -3666,7 +3824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>622</v>
       </c>
@@ -3674,7 +3832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>623</v>
       </c>
@@ -3682,7 +3840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>624</v>
       </c>
@@ -3690,7 +3848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>625</v>
       </c>
@@ -3698,7 +3856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>626</v>
       </c>
@@ -3706,7 +3864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>627</v>
       </c>
@@ -3714,7 +3872,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>628</v>
       </c>
@@ -3722,7 +3880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>629</v>
       </c>
@@ -3730,7 +3888,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>630</v>
       </c>
@@ -3738,7 +3896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>631</v>
       </c>
@@ -3746,7 +3904,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>632</v>
       </c>
@@ -3763,19 +3921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3783,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>701</v>
       </c>
@@ -3791,7 +3949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>702</v>
       </c>
@@ -3799,7 +3957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>703</v>
       </c>
@@ -3807,7 +3965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>704</v>
       </c>
@@ -3815,7 +3973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>705</v>
       </c>
@@ -3823,7 +3981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>706</v>
       </c>
@@ -3831,7 +3989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>707</v>
       </c>
@@ -3839,7 +3997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>708</v>
       </c>
@@ -3847,7 +4005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>709</v>
       </c>
@@ -3855,7 +4013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>710</v>
       </c>
@@ -3863,7 +4021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>711</v>
       </c>
@@ -3871,7 +4029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>717</v>
       </c>
@@ -3879,7 +4037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>718</v>
       </c>
@@ -3887,7 +4045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>719</v>
       </c>
@@ -3895,7 +4053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>720</v>
       </c>
@@ -3903,7 +4061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>721</v>
       </c>
@@ -3911,7 +4069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>722</v>
       </c>
@@ -3919,7 +4077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>723</v>
       </c>
@@ -3927,7 +4085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>724</v>
       </c>
@@ -3935,7 +4093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>725</v>
       </c>
@@ -3943,7 +4101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>726</v>
       </c>
@@ -3951,7 +4109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>727</v>
       </c>
@@ -3959,7 +4117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>728</v>
       </c>
@@ -3967,7 +4125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>729</v>
       </c>
@@ -3975,7 +4133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>730</v>
       </c>
@@ -3983,7 +4141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>731</v>
       </c>
@@ -3991,7 +4149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>732</v>
       </c>
@@ -3999,7 +4157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>775</v>
       </c>
@@ -4007,7 +4165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>776</v>
       </c>
@@ -4015,7 +4173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>777</v>
       </c>
@@ -4023,7 +4181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>778</v>
       </c>
@@ -4031,7 +4189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>779</v>
       </c>
@@ -4048,19 +4206,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4068,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>801</v>
       </c>
@@ -4076,7 +4234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>802</v>
       </c>
@@ -4084,7 +4242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>803</v>
       </c>
@@ -4092,7 +4250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>804</v>
       </c>
@@ -4100,7 +4258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>805</v>
       </c>
@@ -4108,7 +4266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>806</v>
       </c>
@@ -4116,7 +4274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>807</v>
       </c>
@@ -4124,7 +4282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>808</v>
       </c>
@@ -4132,7 +4290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>809</v>
       </c>
@@ -4140,7 +4298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>810</v>
       </c>
@@ -4148,7 +4306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>811</v>
       </c>
@@ -4156,7 +4314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>812</v>
       </c>
@@ -4164,7 +4322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>813</v>
       </c>
@@ -4172,7 +4330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>814</v>
       </c>
@@ -4180,7 +4338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>815</v>
       </c>
@@ -4188,7 +4346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>816</v>
       </c>
@@ -4196,7 +4354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>817</v>
       </c>
@@ -4204,7 +4362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>818</v>
       </c>
@@ -4212,7 +4370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>819</v>
       </c>
@@ -4220,7 +4378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>820</v>
       </c>
@@ -4228,7 +4386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>821</v>
       </c>
@@ -4236,7 +4394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>822</v>
       </c>
@@ -4244,7 +4402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>823</v>
       </c>
@@ -4252,7 +4410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>824</v>
       </c>
@@ -4260,7 +4418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>825</v>
       </c>
@@ -4268,7 +4426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>826</v>
       </c>
@@ -4276,7 +4434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>827</v>
       </c>
@@ -4284,7 +4442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>828</v>
       </c>
@@ -4292,7 +4450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>829</v>
       </c>
@@ -4300,7 +4458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>830</v>
       </c>
@@ -4308,7 +4466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>831</v>
       </c>
@@ -4316,7 +4474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>832</v>
       </c>

</xml_diff>